<commit_message>
evaluate model for metadata finished
</commit_message>
<xml_diff>
--- a/out/extracted_metadata.xlsx
+++ b/out/extracted_metadata.xlsx
@@ -552,7 +552,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>24219576</t>
+          <t>24219576 1.1. Foie</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -626,7 +626,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>24BB11466</t>
+          <t>24BB11466 07</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -774,7 +774,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>24MH9794</t>
+          <t>24MH9794 RF</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -811,7 +811,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>24MH9721</t>
+          <t>24MH9721 BN</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -848,7 +848,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>24EC09559</t>
+          <t>24EC09559 frottis 1</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -922,7 +922,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>24CU052383</t>
+          <t>24CU052383 pneu</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">

</xml_diff>